<commit_message>
Mis a jour 29/03/2020
</commit_message>
<xml_diff>
--- a/Bilan Entrées Sorties.xlsx
+++ b/Bilan Entrées Sorties.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wassim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mes_Projets\ProjetElectro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E43911-C4FD-40A1-A45D-C71F4BD23B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F5B68025-E6B7-4BB6-AE7A-38AD680CA839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -232,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,6 +414,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -428,9 +430,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -746,62 +745,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB785BF-D0E6-4681-8779-0376D60BC8EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -821,7 +820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -841,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -861,7 +860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -873,7 +872,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -885,7 +884,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>9</v>
       </c>
@@ -898,14 +897,14 @@
       <c r="D13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
@@ -925,7 +924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -937,7 +936,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -949,7 +948,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>11</v>
       </c>
@@ -969,7 +968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -981,7 +980,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>37</v>
       </c>
@@ -994,14 +993,14 @@
       <c r="D19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>43</v>
       </c>
@@ -1074,14 +1073,14 @@
       <c r="D23" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>43</v>
       </c>
@@ -1094,10 +1093,10 @@
       <c r="D24" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>43</v>
       </c>
@@ -1109,7 +1108,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>43</v>
       </c>
@@ -1121,7 +1120,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>49</v>
       </c>
@@ -1134,14 +1133,14 @@
       <c r="D27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>49</v>
       </c>
@@ -1154,12 +1153,12 @@
       <c r="D28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="20"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>49</v>
       </c>
@@ -1197,7 +1196,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>49</v>
       </c>
@@ -1217,7 +1216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>49</v>
       </c>
@@ -1237,7 +1236,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>49</v>
       </c>
@@ -1249,7 +1248,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>49</v>
       </c>
@@ -1261,7 +1260,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>57</v>
       </c>

</xml_diff>